<commit_message>
send requested data to 1 user only
</commit_message>
<xml_diff>
--- a/test/test_data.xlsx
+++ b/test/test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\xampp\htdocs\shiptrack\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\My Projects\python\tracker\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5176A833-CD7D-4943-976A-7ED49319EEA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B2E8B0-F936-47E0-9E39-EA111AC1A741}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{FA74C35B-7219-43C9-8E04-E7F52C939C48}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{FA74C35B-7219-43C9-8E04-E7F52C939C48}"/>
   </bookViews>
   <sheets>
     <sheet name="tactical_figure" sheetId="1" r:id="rId1"/>
@@ -812,11 +812,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E11DA0-4C9C-4C30-9126-693F30353463}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A11"/>
+      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="R4" t="s">
         <v>25</v>
@@ -1440,7 +1440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5386DC-0A0F-494A-BC9D-1E8882C58A03}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>